<commit_message>
Alteração da listagem dos dados de um Agente. Listagem das multas, viaturas e condutores. Alteração das definições dos modelos para permitirem o "lazy loading".
</commit_message>
<xml_diff>
--- a/Multas/Multas/multas (1).xlsx
+++ b/Multas/Multas/multas (1).xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcasimiro\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B1A07C-3579-4CA2-A118-F98D68137CC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BC881CFE-C9ED-4F07-B108-CBC026CEF07F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Agentes" sheetId="3" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="Condutores" sheetId="5" r:id="rId3"/>
     <sheet name="Multas" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -960,7 +954,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1335,14 +1329,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42195F75-012E-42DB-92FD-B610538BD49D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1597,7 +1591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8419AC-8980-46A8-97BB-340C841F7948}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2388,7 +2382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3C40BE-8518-4E27-9A0E-513995612307}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2477,7 +2471,7 @@
       </c>
       <c r="E4" t="str">
         <f ca="1">"9"&amp;RANDBETWEEN(1,3)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>937807523</v>
+        <v>912704217</v>
       </c>
       <c r="F4" s="1">
         <v>23794</v>
@@ -2494,15 +2488,15 @@
       </c>
       <c r="J4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="K4">
         <f ca="1">RANDBETWEEN(1,28)</f>
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="M4" t="str">
         <f ca="1">"   new Condutores {"&amp;B$3&amp;"="&amp;B4&amp;", "&amp;C$3&amp;"="""&amp;C4&amp;""", "&amp;D$3&amp;"="""&amp;D4&amp;""", "&amp;E$3&amp;"="""&amp;E4&amp;""", "&amp;F$3&amp;"=new DateTime("&amp;YEAR(F4)&amp;","&amp;MONTH(F4)&amp;","&amp;DAY(F4)&amp;"), "&amp;G$3&amp;"="""&amp;G4&amp;""", "&amp;H$3&amp;"="""&amp;H4&amp;""", "&amp;I$3&amp;"=new DateTime("&amp;I4&amp;","&amp;J4&amp;","&amp;K4&amp;") },"</f>
-        <v xml:space="preserve">   new Condutores {ID=1, Nome=" João Santos", BI="123456", Telemovel="937807523", DataNascimento=new DateTime(1965,2,21), NumCartaConducao="SA-12345", LocalEmissao="Santarém", DataValidadeCarta=new DateTime(2029,11,14) },</v>
+        <v xml:space="preserve">   new Condutores {ID=1, Nome=" João Santos", BI="123456", Telemovel="912704217", DataNascimento=new DateTime(1965,2,21), NumCartaConducao="SA-12345", LocalEmissao="Santarém", DataValidadeCarta=new DateTime(2029,5,23) },</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -2517,7 +2511,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" ref="E5:E40" ca="1" si="0">"9"&amp;RANDBETWEEN(1,3)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>933962058</v>
+        <v>913604436</v>
       </c>
       <c r="F5" s="1">
         <v>24307</v>
@@ -2530,19 +2524,19 @@
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I40" ca="1" si="1">RANDBETWEEN(2019,2030)</f>
-        <v>2019</v>
+        <v>2027</v>
       </c>
       <c r="J5">
         <f t="shared" ref="J5:J40" ca="1" si="2">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K40" ca="1" si="3">RANDBETWEEN(1,28)</f>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ref="M5:M39" ca="1" si="4">"   new Condutores {"&amp;B$3&amp;"="&amp;B5&amp;", "&amp;C$3&amp;"="""&amp;C5&amp;""", "&amp;D$3&amp;"="""&amp;D5&amp;""", "&amp;E$3&amp;"="""&amp;E5&amp;""", "&amp;F$3&amp;"=new DateTime("&amp;YEAR(F5)&amp;","&amp;MONTH(F5)&amp;","&amp;DAY(F5)&amp;"), "&amp;G$3&amp;"="""&amp;G5&amp;""", "&amp;H$3&amp;"="""&amp;H5&amp;""", "&amp;I$3&amp;"=new DateTime("&amp;I5&amp;","&amp;J5&amp;","&amp;K5&amp;") },"</f>
-        <v xml:space="preserve">   new Condutores {ID=2, Nome=" Daniel Soares", BI="259608283", Telemovel="933962058", DataNascimento=new DateTime(1966,7,19), NumCartaConducao="LX-244056", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2019,3,18) },</v>
+        <v xml:space="preserve">   new Condutores {ID=2, Nome=" Daniel Soares", BI="259608283", Telemovel="913604436", DataNascimento=new DateTime(1966,7,19), NumCartaConducao="LX-244056", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2027,8,13) },</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -2557,7 +2551,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>914150064</v>
+        <v>936765184</v>
       </c>
       <c r="F6" s="1">
         <v>29923</v>
@@ -2570,19 +2564,19 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=3, Nome=" Adriana Rodrigues", BI="588141871", Telemovel="914150064", DataNascimento=new DateTime(1981,12,3), NumCartaConducao="LX-847226", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2022,4,18) },</v>
+        <v xml:space="preserve">   new Condutores {ID=3, Nome=" Adriana Rodrigues", BI="588141871", Telemovel="936765184", DataNascimento=new DateTime(1981,12,3), NumCartaConducao="LX-847226", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2023,8,5) },</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -2597,7 +2591,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>915071667</v>
+        <v>910800871</v>
       </c>
       <c r="F7" s="1">
         <v>28392</v>
@@ -2614,15 +2608,15 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=4, Nome=" Rosa Fernandes", BI="728246437", Telemovel="915071667", DataNascimento=new DateTime(1977,9,24), NumCartaConducao="SA-89573", LocalEmissao="Santarém", DataValidadeCarta=new DateTime(2020,6,24) },</v>
+        <v xml:space="preserve">   new Condutores {ID=4, Nome=" Rosa Fernandes", BI="728246437", Telemovel="910800871", DataNascimento=new DateTime(1977,9,24), NumCartaConducao="SA-89573", LocalEmissao="Santarém", DataValidadeCarta=new DateTime(2020,10,15) },</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2637,7 +2631,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>934951594</v>
+        <v>925274012</v>
       </c>
       <c r="F8" s="1">
         <v>19588</v>
@@ -2650,19 +2644,19 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=5, Nome=" Carolina Oliveira", BI="858156342", Telemovel="934951594", DataNascimento=new DateTime(1953,8,17), NumCartaConducao="AC-738163", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2025,8,10) },</v>
+        <v xml:space="preserve">   new Condutores {ID=5, Nome=" Carolina Oliveira", BI="858156342", Telemovel="925274012", DataNascimento=new DateTime(1953,8,17), NumCartaConducao="AC-738163", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2023,12,16) },</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
@@ -2677,7 +2671,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>919710991</v>
+        <v>910156824</v>
       </c>
       <c r="F9" s="1">
         <v>23611</v>
@@ -2690,7 +2684,7 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="1"/>
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="2"/>
@@ -2698,11 +2692,11 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=6, Nome=" César Sousa", BI="507261086", Telemovel="919710991", DataNascimento=new DateTime(1964,8,22), NumCartaConducao="FA-321287", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2029,3,27) },</v>
+        <v xml:space="preserve">   new Condutores {ID=6, Nome=" César Sousa", BI="507261086", Telemovel="910156824", DataNascimento=new DateTime(1964,8,22), NumCartaConducao="FA-321287", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2027,3,22) },</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -2717,7 +2711,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>923175076</v>
+        <v>922399465</v>
       </c>
       <c r="F10" s="1">
         <v>20537</v>
@@ -2730,19 +2724,19 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="1"/>
-        <v>2019</v>
+        <v>2025</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=7, Nome=" Maria Teixeira", BI="618881552", Telemovel="923175076", DataNascimento=new DateTime(1956,3,23), NumCartaConducao="BE-782268", LocalEmissao="Beja", DataValidadeCarta=new DateTime(2019,12,27) },</v>
+        <v xml:space="preserve">   new Condutores {ID=7, Nome=" Maria Teixeira", BI="618881552", Telemovel="922399465", DataNascimento=new DateTime(1956,3,23), NumCartaConducao="BE-782268", LocalEmissao="Beja", DataValidadeCarta=new DateTime(2025,7,6) },</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -2757,7 +2751,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>921625167</v>
+        <v>921785848</v>
       </c>
       <c r="F11" s="1">
         <v>20414</v>
@@ -2770,19 +2764,19 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="1"/>
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=8, Nome=" Maria Melo", BI="819229141", Telemovel="921625167", DataNascimento=new DateTime(1955,11,21), NumCartaConducao="EV-409189", LocalEmissao="Évora", DataValidadeCarta=new DateTime(2024,1,13) },</v>
+        <v xml:space="preserve">   new Condutores {ID=8, Nome=" Maria Melo", BI="819229141", Telemovel="921785848", DataNascimento=new DateTime(1955,11,21), NumCartaConducao="EV-409189", LocalEmissao="Évora", DataValidadeCarta=new DateTime(2021,12,28) },</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -2797,7 +2791,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>926541822</v>
+        <v>930088271</v>
       </c>
       <c r="F12" s="1">
         <v>23966</v>
@@ -2810,19 +2804,19 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="1"/>
-        <v>2027</v>
+        <v>2023</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=9, Nome=" Francisco Vieira", BI="468921645", Telemovel="926541822", DataNascimento=new DateTime(1965,8,12), NumCartaConducao="PO-26600", LocalEmissao="Porto", DataValidadeCarta=new DateTime(2027,11,28) },</v>
+        <v xml:space="preserve">   new Condutores {ID=9, Nome=" Francisco Vieira", BI="468921645", Telemovel="930088271", DataNascimento=new DateTime(1965,8,12), NumCartaConducao="PO-26600", LocalEmissao="Porto", DataValidadeCarta=new DateTime(2023,3,13) },</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -2837,7 +2831,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>916813865</v>
+        <v>922007012</v>
       </c>
       <c r="F13" s="1">
         <v>13746</v>
@@ -2854,15 +2848,15 @@
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=10, Nome=" Leonardo Marques", BI="110562475", Telemovel="916813865", DataNascimento=new DateTime(1937,8,19), NumCartaConducao="AC-488808", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2023,3,18) },</v>
+        <v xml:space="preserve">   new Condutores {ID=10, Nome=" Leonardo Marques", BI="110562475", Telemovel="922007012", DataNascimento=new DateTime(1937,8,19), NumCartaConducao="AC-488808", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2023,2,4) },</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -2877,7 +2871,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>932400873</v>
+        <v>932952485</v>
       </c>
       <c r="F14" s="1">
         <v>28221</v>
@@ -2890,19 +2884,19 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>2028</v>
+        <v>2024</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=11, Nome=" Fábio Carvalho", BI="241857636", Telemovel="932400873", DataNascimento=new DateTime(1977,4,6), NumCartaConducao="EV-196487", LocalEmissao="Évora", DataValidadeCarta=new DateTime(2028,1,25) },</v>
+        <v xml:space="preserve">   new Condutores {ID=11, Nome=" Fábio Carvalho", BI="241857636", Telemovel="932952485", DataNascimento=new DateTime(1977,4,6), NumCartaConducao="EV-196487", LocalEmissao="Évora", DataValidadeCarta=new DateTime(2024,7,14) },</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
@@ -2917,7 +2911,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>924168781</v>
+        <v>924867916</v>
       </c>
       <c r="F15" s="1">
         <v>16714</v>
@@ -2930,19 +2924,19 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="1"/>
-        <v>2029</v>
+        <v>2020</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=12, Nome=" Tiago Vieira", BI="192262426", Telemovel="924168781", DataNascimento=new DateTime(1945,10,4), NumCartaConducao="EV-115244", LocalEmissao="Évora", DataValidadeCarta=new DateTime(2029,5,1) },</v>
+        <v xml:space="preserve">   new Condutores {ID=12, Nome=" Tiago Vieira", BI="192262426", Telemovel="924867916", DataNascimento=new DateTime(1945,10,4), NumCartaConducao="EV-115244", LocalEmissao="Évora", DataValidadeCarta=new DateTime(2020,10,6) },</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
@@ -2957,7 +2951,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>939639959</v>
+        <v>914725327</v>
       </c>
       <c r="F16" s="1">
         <v>18722</v>
@@ -2970,19 +2964,19 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="1"/>
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=13, Nome=" Rosana Soares", BI="233334917", Telemovel="939639959", DataNascimento=new DateTime(1951,4,4), NumCartaConducao="EV-257116", LocalEmissao="Évora", DataValidadeCarta=new DateTime(2028,4,15) },</v>
+        <v xml:space="preserve">   new Condutores {ID=13, Nome=" Rosana Soares", BI="233334917", Telemovel="914725327", DataNascimento=new DateTime(1951,4,4), NumCartaConducao="EV-257116", LocalEmissao="Évora", DataValidadeCarta=new DateTime(2027,8,23) },</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
@@ -2997,7 +2991,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>925415394</v>
+        <v>930310907</v>
       </c>
       <c r="F17" s="1">
         <v>31162</v>
@@ -3010,19 +3004,19 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>2026</v>
+        <v>2020</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=14, Nome=" Rui Freitas", BI="251617767", Telemovel="925415394", DataNascimento=new DateTime(1985,4,25), NumCartaConducao="PO-611668", LocalEmissao="Porto", DataValidadeCarta=new DateTime(2026,6,1) },</v>
+        <v xml:space="preserve">   new Condutores {ID=14, Nome=" Rui Freitas", BI="251617767", Telemovel="930310907", DataNascimento=new DateTime(1985,4,25), NumCartaConducao="PO-611668", LocalEmissao="Porto", DataValidadeCarta=new DateTime(2020,10,26) },</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -3037,7 +3031,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>917701936</v>
+        <v>921513904</v>
       </c>
       <c r="F18" s="1">
         <v>22619</v>
@@ -3050,19 +3044,19 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>2028</v>
+        <v>2024</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=15, Nome=" César Soares", BI="151965324", Telemovel="917701936", DataNascimento=new DateTime(1961,12,4), NumCartaConducao="VI-815500", LocalEmissao="Viseu", DataValidadeCarta=new DateTime(2028,2,12) },</v>
+        <v xml:space="preserve">   new Condutores {ID=15, Nome=" César Soares", BI="151965324", Telemovel="921513904", DataNascimento=new DateTime(1961,12,4), NumCartaConducao="VI-815500", LocalEmissao="Viseu", DataValidadeCarta=new DateTime(2024,9,1) },</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -3077,7 +3071,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>927571282</v>
+        <v>912669560</v>
       </c>
       <c r="F19" s="1">
         <v>26096</v>
@@ -3090,19 +3084,19 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=16, Nome=" Márcio Sousa", BI="74975648", Telemovel="927571282", DataNascimento=new DateTime(1971,6,12), NumCartaConducao="AC-680776", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2023,1,28) },</v>
+        <v xml:space="preserve">   new Condutores {ID=16, Nome=" Márcio Sousa", BI="74975648", Telemovel="912669560", DataNascimento=new DateTime(1971,6,12), NumCartaConducao="AC-680776", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2019,9,13) },</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
@@ -3117,7 +3111,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>923590106</v>
+        <v>916499427</v>
       </c>
       <c r="F20" s="1">
         <v>26987</v>
@@ -3130,19 +3124,19 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>2029</v>
+        <v>2020</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=17, Nome=" Eduardo Vieira", BI="254872277", Telemovel="923590106", DataNascimento=new DateTime(1973,11,19), NumCartaConducao="FA-812863", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2029,1,20) },</v>
+        <v xml:space="preserve">   new Condutores {ID=17, Nome=" Eduardo Vieira", BI="254872277", Telemovel="916499427", DataNascimento=new DateTime(1973,11,19), NumCartaConducao="FA-812863", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2020,3,9) },</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -3157,7 +3151,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>928909338</v>
+        <v>911186838</v>
       </c>
       <c r="F21" s="1">
         <v>18522</v>
@@ -3170,19 +3164,19 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=18, Nome=" Adriana Oliveira", BI="686190303", Telemovel="928909338", DataNascimento=new DateTime(1950,9,16), NumCartaConducao="BE-100918", LocalEmissao="Beja", DataValidadeCarta=new DateTime(2023,9,25) },</v>
+        <v xml:space="preserve">   new Condutores {ID=18, Nome=" Adriana Oliveira", BI="686190303", Telemovel="911186838", DataNascimento=new DateTime(1950,9,16), NumCartaConducao="BE-100918", LocalEmissao="Beja", DataValidadeCarta=new DateTime(2020,10,8) },</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -3197,7 +3191,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>917671684</v>
+        <v>911311968</v>
       </c>
       <c r="F22" s="1">
         <v>31053</v>
@@ -3214,15 +3208,15 @@
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=19, Nome=" Beatriz Soares", BI="163679850", Telemovel="917671684", DataNascimento=new DateTime(1985,1,6), NumCartaConducao="AC-374173", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2022,5,3) },</v>
+        <v xml:space="preserve">   new Condutores {ID=19, Nome=" Beatriz Soares", BI="163679850", Telemovel="911311968", DataNascimento=new DateTime(1985,1,6), NumCartaConducao="AC-374173", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2022,4,16) },</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
@@ -3237,7 +3231,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>935528953</v>
+        <v>921730428</v>
       </c>
       <c r="F23" s="1">
         <v>20991</v>
@@ -3250,19 +3244,19 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>2019</v>
+        <v>2027</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=20, Nome=" Adriana Sousa", BI="845941950", Telemovel="935528953", DataNascimento=new DateTime(1957,6,20), NumCartaConducao="MA-107861", LocalEmissao="Madeira", DataValidadeCarta=new DateTime(2019,4,3) },</v>
+        <v xml:space="preserve">   new Condutores {ID=20, Nome=" Adriana Sousa", BI="845941950", Telemovel="921730428", DataNascimento=new DateTime(1957,6,20), NumCartaConducao="MA-107861", LocalEmissao="Madeira", DataValidadeCarta=new DateTime(2027,9,25) },</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
@@ -3277,7 +3271,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>938406022</v>
+        <v>936619038</v>
       </c>
       <c r="F24" s="1">
         <v>12529</v>
@@ -3290,19 +3284,19 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>2028</v>
+        <v>2023</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=21, Nome=" Patrícia Gonçalves", BI="185717766", Telemovel="938406022", DataNascimento=new DateTime(1934,4,20), NumCartaConducao="MA-949155", LocalEmissao="Madeira", DataValidadeCarta=new DateTime(2028,5,14) },</v>
+        <v xml:space="preserve">   new Condutores {ID=21, Nome=" Patrícia Gonçalves", BI="185717766", Telemovel="936619038", DataNascimento=new DateTime(1934,4,20), NumCartaConducao="MA-949155", LocalEmissao="Madeira", DataValidadeCarta=new DateTime(2023,3,22) },</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
@@ -3317,7 +3311,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>917218249</v>
+        <v>936866963</v>
       </c>
       <c r="F25" s="1">
         <v>30992</v>
@@ -3330,19 +3324,19 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>2019</v>
+        <v>2025</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=22, Nome=" Paula Martins", BI="782184726", Telemovel="917218249", DataNascimento=new DateTime(1984,11,6), NumCartaConducao="BE-743939", LocalEmissao="Beja", DataValidadeCarta=new DateTime(2019,1,7) },</v>
+        <v xml:space="preserve">   new Condutores {ID=22, Nome=" Paula Martins", BI="782184726", Telemovel="936866963", DataNascimento=new DateTime(1984,11,6), NumCartaConducao="BE-743939", LocalEmissao="Beja", DataValidadeCarta=new DateTime(2025,5,1) },</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
@@ -3357,7 +3351,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>929706685</v>
+        <v>936401481</v>
       </c>
       <c r="F26" s="1">
         <v>24770</v>
@@ -3370,19 +3364,19 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=23, Nome=" Andreia Vieira", BI="994307613", Telemovel="929706685", DataNascimento=new DateTime(1967,10,25), NumCartaConducao="FA-165555", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2022,10,24) },</v>
+        <v xml:space="preserve">   new Condutores {ID=23, Nome=" Andreia Vieira", BI="994307613", Telemovel="936401481", DataNascimento=new DateTime(1967,10,25), NumCartaConducao="FA-165555", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2024,11,3) },</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
@@ -3397,7 +3391,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>924606729</v>
+        <v>935145551</v>
       </c>
       <c r="F27" s="1">
         <v>12261</v>
@@ -3410,19 +3404,19 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=24, Nome=" Elisabete Morais", BI="270424301", Telemovel="924606729", DataNascimento=new DateTime(1933,7,26), NumCartaConducao="FA-583994", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2026,6,1) },</v>
+        <v xml:space="preserve">   new Condutores {ID=24, Nome=" Elisabete Morais", BI="270424301", Telemovel="935145551", DataNascimento=new DateTime(1933,7,26), NumCartaConducao="FA-583994", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2025,2,2) },</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
@@ -3437,7 +3431,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>926269929</v>
+        <v>915760080</v>
       </c>
       <c r="F28" s="1">
         <v>13710</v>
@@ -3450,19 +3444,19 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=25, Nome=" Marlene Melo", BI="270120676", Telemovel="926269929", DataNascimento=new DateTime(1937,7,14), NumCartaConducao="FA-751427", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2023,10,3) },</v>
+        <v xml:space="preserve">   new Condutores {ID=25, Nome=" Marlene Melo", BI="270120676", Telemovel="915760080", DataNascimento=new DateTime(1937,7,14), NumCartaConducao="FA-751427", LocalEmissao="Faro", DataValidadeCarta=new DateTime(2022,7,11) },</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
@@ -3477,7 +3471,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>925808359</v>
+        <v>933588295</v>
       </c>
       <c r="F29" s="1">
         <v>15392</v>
@@ -3490,19 +3484,19 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=26, Nome=" Marlene Pinto", BI="751512767", Telemovel="925808359", DataNascimento=new DateTime(1942,2,20), NumCartaConducao="LX-963025", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2028,5,10) },</v>
+        <v xml:space="preserve">   new Condutores {ID=26, Nome=" Marlene Pinto", BI="751512767", Telemovel="933588295", DataNascimento=new DateTime(1942,2,20), NumCartaConducao="LX-963025", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2030,10,28) },</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
@@ -3517,7 +3511,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>918536695</v>
+        <v>914228977</v>
       </c>
       <c r="F30" s="1">
         <v>24546</v>
@@ -3530,19 +3524,19 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="1"/>
-        <v>2029</v>
+        <v>2020</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=27, Nome=" Luís Lopes", BI="497555127", Telemovel="918536695", DataNascimento=new DateTime(1967,3,15), NumCartaConducao="MA-512423", LocalEmissao="Madeira", DataValidadeCarta=new DateTime(2029,6,20) },</v>
+        <v xml:space="preserve">   new Condutores {ID=27, Nome=" Luís Lopes", BI="497555127", Telemovel="914228977", DataNascimento=new DateTime(1967,3,15), NumCartaConducao="MA-512423", LocalEmissao="Madeira", DataValidadeCarta=new DateTime(2020,10,4) },</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
@@ -3557,7 +3551,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>918872130</v>
+        <v>926126097</v>
       </c>
       <c r="F31" s="1">
         <v>28273</v>
@@ -3570,19 +3564,19 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="1"/>
-        <v>2020</v>
+        <v>2026</v>
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=28, Nome=" Denise Vieira", BI="264427182", Telemovel="918872130", DataNascimento=new DateTime(1977,5,28), NumCartaConducao="PO-887507", LocalEmissao="Porto", DataValidadeCarta=new DateTime(2020,5,4) },</v>
+        <v xml:space="preserve">   new Condutores {ID=28, Nome=" Denise Vieira", BI="264427182", Telemovel="926126097", DataNascimento=new DateTime(1977,5,28), NumCartaConducao="PO-887507", LocalEmissao="Porto", DataValidadeCarta=new DateTime(2026,9,10) },</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
@@ -3597,7 +3591,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>938446983</v>
+        <v>913755484</v>
       </c>
       <c r="F32" s="1">
         <v>22208</v>
@@ -3610,11 +3604,11 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="1"/>
-        <v>2024</v>
+        <v>2027</v>
       </c>
       <c r="J32">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="3"/>
@@ -3622,7 +3616,7 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=29, Nome=" Cristina Rosa", BI="461453252", Telemovel="938446983", DataNascimento=new DateTime(1960,10,19), NumCartaConducao="MA-257694", LocalEmissao="Madeira", DataValidadeCarta=new DateTime(2024,2,21) },</v>
+        <v xml:space="preserve">   new Condutores {ID=29, Nome=" Cristina Rosa", BI="461453252", Telemovel="913755484", DataNascimento=new DateTime(1960,10,19), NumCartaConducao="MA-257694", LocalEmissao="Madeira", DataValidadeCarta=new DateTime(2027,1,21) },</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
@@ -3637,7 +3631,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>916459437</v>
+        <v>920513126</v>
       </c>
       <c r="F33" s="1">
         <v>15464</v>
@@ -3650,19 +3644,19 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="1"/>
-        <v>2020</v>
+        <v>2028</v>
       </c>
       <c r="J33">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=30, Nome=" Carmem Lopes", BI="91728054", Telemovel="916459437", DataNascimento=new DateTime(1942,5,3), NumCartaConducao="SA-324795", LocalEmissao="Santarém", DataValidadeCarta=new DateTime(2020,5,23) },</v>
+        <v xml:space="preserve">   new Condutores {ID=30, Nome=" Carmem Lopes", BI="91728054", Telemovel="920513126", DataNascimento=new DateTime(1942,5,3), NumCartaConducao="SA-324795", LocalEmissao="Santarém", DataValidadeCarta=new DateTime(2028,3,24) },</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
@@ -3677,7 +3671,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>913238451</v>
+        <v>918693900</v>
       </c>
       <c r="F34" s="1">
         <v>20615</v>
@@ -3690,19 +3684,19 @@
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="1"/>
-        <v>2027</v>
+        <v>2020</v>
       </c>
       <c r="J34">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K34">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=31, Nome=" Rosana Carvalho", BI="279887145", Telemovel="913238451", DataNascimento=new DateTime(1956,6,9), NumCartaConducao="LX-182393", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2027,9,7) },</v>
+        <v xml:space="preserve">   new Condutores {ID=31, Nome=" Rosana Carvalho", BI="279887145", Telemovel="918693900", DataNascimento=new DateTime(1956,6,9), NumCartaConducao="LX-182393", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2020,8,25) },</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -3717,7 +3711,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>924025641</v>
+        <v>926472173</v>
       </c>
       <c r="F35" s="1">
         <v>26446</v>
@@ -3734,15 +3728,15 @@
       </c>
       <c r="J35">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K35">
         <f t="shared" ca="1" si="3"/>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=32, Nome=" Paula Silva", BI="372845332", Telemovel="924025641", DataNascimento=new DateTime(1972,5,27), NumCartaConducao="VI-966301", LocalEmissao="Viseu", DataValidadeCarta=new DateTime(2019,12,21) },</v>
+        <v xml:space="preserve">   new Condutores {ID=32, Nome=" Paula Silva", BI="372845332", Telemovel="926472173", DataNascimento=new DateTime(1972,5,27), NumCartaConducao="VI-966301", LocalEmissao="Viseu", DataValidadeCarta=new DateTime(2019,5,14) },</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
@@ -3757,7 +3751,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>917974452</v>
+        <v>926676031</v>
       </c>
       <c r="F36" s="1">
         <v>27944</v>
@@ -3770,19 +3764,19 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
-        <v>2021</v>
+        <v>2028</v>
       </c>
       <c r="J36">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K36">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=33, Nome=" Mara Vieira", BI="682215833", Telemovel="917974452", DataNascimento=new DateTime(1976,7,3), NumCartaConducao="LX-753375", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2021,2,23) },</v>
+        <v xml:space="preserve">   new Condutores {ID=33, Nome=" Mara Vieira", BI="682215833", Telemovel="926676031", DataNascimento=new DateTime(1976,7,3), NumCartaConducao="LX-753375", LocalEmissao="Lisboa", DataValidadeCarta=new DateTime(2028,1,13) },</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -3797,7 +3791,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>933754879</v>
+        <v>934392582</v>
       </c>
       <c r="F37" s="1">
         <v>12325</v>
@@ -3810,7 +3804,7 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="1"/>
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="J37">
         <f t="shared" ca="1" si="2"/>
@@ -3818,11 +3812,11 @@
       </c>
       <c r="K37">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=34, Nome=" Adão Pinto", BI="263833191", Telemovel="933754879", DataNascimento=new DateTime(1933,9,28), NumCartaConducao="AC-380383", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2021,7,8) },</v>
+        <v xml:space="preserve">   new Condutores {ID=34, Nome=" Adão Pinto", BI="263833191", Telemovel="934392582", DataNascimento=new DateTime(1933,9,28), NumCartaConducao="AC-380383", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2024,7,2) },</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
@@ -3837,7 +3831,7 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>927245264</v>
+        <v>922223704</v>
       </c>
       <c r="F38" s="1">
         <v>14657</v>
@@ -3850,19 +3844,19 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="1"/>
-        <v>2020</v>
+        <v>2025</v>
       </c>
       <c r="J38">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K38">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=35, Nome=" Daniel Rodrigues", BI="785025953", Telemovel="927245264", DataNascimento=new DateTime(1940,2,16), NumCartaConducao="BE-173356", LocalEmissao="Beja", DataValidadeCarta=new DateTime(2020,7,5) },</v>
+        <v xml:space="preserve">   new Condutores {ID=35, Nome=" Daniel Rodrigues", BI="785025953", Telemovel="922223704", DataNascimento=new DateTime(1940,2,16), NumCartaConducao="BE-173356", LocalEmissao="Beja", DataValidadeCarta=new DateTime(2025,3,8) },</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
@@ -3877,7 +3871,7 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>918038910</v>
+        <v>935828552</v>
       </c>
       <c r="F39" s="1">
         <v>11895</v>
@@ -3890,19 +3884,19 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="1"/>
-        <v>2024</v>
+        <v>2027</v>
       </c>
       <c r="J39">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K39">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">   new Condutores {ID=36, Nome=" Sandra Rodrigues", BI="639730253", Telemovel="918038910", DataNascimento=new DateTime(1932,7,25), NumCartaConducao="AC-232544", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2024,1,2) },</v>
+        <v xml:space="preserve">   new Condutores {ID=36, Nome=" Sandra Rodrigues", BI="639730253", Telemovel="935828552", DataNascimento=new DateTime(1932,7,25), NumCartaConducao="AC-232544", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2027,7,15) },</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
@@ -3917,7 +3911,7 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>924584920</v>
+        <v>935910948</v>
       </c>
       <c r="F40" s="1">
         <v>30043</v>
@@ -3930,19 +3924,19 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="1"/>
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="J40">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K40">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="M40" t="str">
         <f ca="1">"   new Condutores {"&amp;B$3&amp;"="&amp;B40&amp;", "&amp;C$3&amp;"="""&amp;C40&amp;""", "&amp;D$3&amp;"="""&amp;D40&amp;""", "&amp;E$3&amp;"="""&amp;E40&amp;""", "&amp;F$3&amp;"=new DateTime("&amp;YEAR(F40)&amp;","&amp;MONTH(F40)&amp;","&amp;DAY(F40)&amp;"), "&amp;G$3&amp;"="""&amp;G40&amp;""", "&amp;H$3&amp;"="""&amp;H40&amp;""", "&amp;I$3&amp;"=new DateTime("&amp;I40&amp;","&amp;J40&amp;","&amp;K40&amp;") }"</f>
-        <v xml:space="preserve">   new Condutores {ID=37, Nome=" Cláudio Vieira", BI="556447530", Telemovel="924584920", DataNascimento=new DateTime(1982,4,2), NumCartaConducao="AC-488152", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2026,7,17) }</v>
+        <v xml:space="preserve">   new Condutores {ID=37, Nome=" Cláudio Vieira", BI="556447530", Telemovel="935910948", DataNascimento=new DateTime(1982,4,2), NumCartaConducao="AC-488152", LocalEmissao="Açores", DataValidadeCarta=new DateTime(2024,12,9) }</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
@@ -3966,7 +3960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF83BF22-070C-4241-995E-AF2AFDF14BD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6285,7 +6279,7 @@
         <v>10</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" ref="L69:L118" si="1">"   new Multas {"&amp;B$3&amp;"="&amp;B69&amp;", "&amp;C$3&amp;"="""&amp;C69&amp;""", "&amp;D$3&amp;"="""&amp;D69&amp;""", "&amp;E$3&amp;"="&amp;E69&amp;"M, "&amp;F$3&amp;"=new DateTime("&amp;YEAR(F69)+13&amp;","&amp;MONTH(F69)&amp;","&amp;DAY(F69)&amp;"), "&amp;H$3&amp;"="&amp;H69&amp;", "&amp;I$3&amp;"="&amp;I69&amp;", "&amp;J$3&amp;"="&amp;J69&amp;" },"</f>
+        <f t="shared" ref="L69:L117" si="1">"   new Multas {"&amp;B$3&amp;"="&amp;B69&amp;", "&amp;C$3&amp;"="""&amp;C69&amp;""", "&amp;D$3&amp;"="""&amp;D69&amp;""", "&amp;E$3&amp;"="&amp;E69&amp;"M, "&amp;F$3&amp;"=new DateTime("&amp;YEAR(F69)+13&amp;","&amp;MONTH(F69)&amp;","&amp;DAY(F69)&amp;"), "&amp;H$3&amp;"="&amp;H69&amp;", "&amp;I$3&amp;"="&amp;I69&amp;", "&amp;J$3&amp;"="&amp;J69&amp;" },"</f>
         <v xml:space="preserve">   new Multas {ID=42, LocalDaMulta="Lisboa", Infracao="Excesso de velocidade (&gt;20 Km e &lt; 40 Km)", ValorMulta=100.00M, DataDaMulta=new DateTime(2017,6,1), ViaturaFK=19, CondutorFK=14, AgenteFK=10 },</v>
       </c>
     </row>

</xml_diff>